<commit_message>
update projectVelocity and delete TODO file
</commit_message>
<xml_diff>
--- a/ParcodeTaskVelocity.xlsx
+++ b/ParcodeTaskVelocity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\AWb-g4-parcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59064556-D3DE-4771-9FCF-676E340E28C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE6A90-34A7-4389-96EC-CDAF98AE64ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Tâche</t>
   </si>
@@ -141,13 +141,19 @@
   </si>
   <si>
     <t>adaptation pour appareil mobile</t>
+  </si>
+  <si>
+    <t>upvote des commentaires</t>
+  </si>
+  <si>
+    <t>menu arborescent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +164,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -231,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -257,6 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -285,8 +299,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E25" totalsRowShown="0">
-  <autoFilter ref="A1:E25" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E27" totalsRowShown="0">
+  <autoFilter ref="A1:E27" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
     <sortCondition ref="A1:A11"/>
   </sortState>
@@ -600,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7501AF-60F9-49EB-99C2-B40735EA6386}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,10 +734,15 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>1</v>
       </c>
       <c r="E6" s="13"/>
     </row>
@@ -731,10 +750,15 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" t="s">
@@ -758,7 +782,7 @@
       <c r="E8" s="7"/>
       <c r="H8">
         <f>SUM(Tableau1[Task velocity])/COUNT(Tableau1[Task velocity])</f>
-        <v>1.3512396694214877</v>
+        <v>1.2121212121212119</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -797,10 +821,15 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>1</v>
       </c>
       <c r="E11" s="7"/>
     </row>
@@ -808,10 +837,15 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="D12" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -819,10 +853,15 @@
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>1</v>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -830,10 +869,15 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>3</v>
+      </c>
+      <c r="D14" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E14" s="14"/>
     </row>
@@ -841,10 +885,15 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B15">
+        <v>0.25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>1</v>
       </c>
       <c r="E15" s="14"/>
     </row>
@@ -928,10 +977,15 @@
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>2</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -979,6 +1033,29 @@
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v/>
       </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E27" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'dev' into treeView"
This reverts commit b012cc3360f3c9b0035f30b4d9bb0695d2d22f60, reversing
changes made to d4a7d78224b5867332fd55634c789eb5a2335764.
</commit_message>
<xml_diff>
--- a/ParcodeTaskVelocity.xlsx
+++ b/ParcodeTaskVelocity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\AWb-g4-parcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE6A90-34A7-4389-96EC-CDAF98AE64ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59064556-D3DE-4771-9FCF-676E340E28C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Tâche</t>
   </si>
@@ -141,19 +141,13 @@
   </si>
   <si>
     <t>adaptation pour appareil mobile</t>
-  </si>
-  <si>
-    <t>upvote des commentaires</t>
-  </si>
-  <si>
-    <t>menu arborescent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,13 +158,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFC000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -244,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,7 +257,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,8 +285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E27" totalsRowShown="0">
-  <autoFilter ref="A1:E27" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E25" totalsRowShown="0">
+  <autoFilter ref="A1:E25" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
     <sortCondition ref="A1:A11"/>
   </sortState>
@@ -614,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7501AF-60F9-49EB-99C2-B40735EA6386}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,15 +720,10 @@
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+      <c r="C6" s="2"/>
+      <c r="D6" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E6" s="13"/>
     </row>
@@ -750,15 +731,10 @@
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.83333333333333337</v>
+      <c r="C7" s="2"/>
+      <c r="D7" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E7" s="5"/>
       <c r="H7" t="s">
@@ -782,7 +758,7 @@
       <c r="E8" s="7"/>
       <c r="H8">
         <f>SUM(Tableau1[Task velocity])/COUNT(Tableau1[Task velocity])</f>
-        <v>1.2121212121212119</v>
+        <v>1.3512396694214877</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -821,15 +797,10 @@
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+      <c r="C11" s="2"/>
+      <c r="D11" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E11" s="7"/>
     </row>
@@ -837,15 +808,10 @@
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2">
-        <v>3</v>
-      </c>
-      <c r="D12" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.66666666666666663</v>
+      <c r="C12" s="2"/>
+      <c r="D12" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E12" s="7"/>
     </row>
@@ -853,15 +819,10 @@
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+      <c r="C13" s="2"/>
+      <c r="D13" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E13" s="7"/>
     </row>
@@ -869,15 +830,10 @@
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.66666666666666663</v>
+      <c r="C14" s="2"/>
+      <c r="D14" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E14" s="14"/>
     </row>
@@ -885,15 +841,10 @@
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15">
-        <v>0.25</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D15" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+      <c r="C15" s="2"/>
+      <c r="D15" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E15" s="14"/>
     </row>
@@ -977,15 +928,10 @@
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D22" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>2</v>
+      <c r="C22" s="2"/>
+      <c r="D22" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -1033,29 +979,6 @@
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v/>
       </c>
-      <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
-      </c>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
-      </c>
-      <c r="E27" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
travail design / uX : -mise a jour fonctionnelle du footer
</commit_message>
<xml_diff>
--- a/ParcodeTaskVelocity.xlsx
+++ b/ParcodeTaskVelocity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\AWb-g4-parcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FE6A90-34A7-4389-96EC-CDAF98AE64ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8300FA-B68B-414A-B568-F4F102A30F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Tâche</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>menu arborescent</t>
+  </si>
+  <si>
+    <t>au moins 3</t>
+  </si>
+  <si>
+    <t>au moins 4</t>
+  </si>
+  <si>
+    <t>déjà 2</t>
   </si>
 </sst>
 </file>
@@ -617,21 +626,21 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -679,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -698,7 +707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -714,7 +723,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -730,7 +739,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -746,7 +755,7 @@
       </c>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -765,7 +774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -785,7 +794,7 @@
         <v>1.2121212121212119</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -801,7 +810,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -817,7 +826,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -833,7 +842,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -849,7 +858,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -865,7 +874,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -881,7 +890,7 @@
       </c>
       <c r="E14" s="14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -897,7 +906,7 @@
       </c>
       <c r="E15" s="14"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -908,7 +917,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -924,7 +933,7 @@
       </c>
       <c r="E17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -940,10 +949,13 @@
       </c>
       <c r="E18" s="7"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="10" t="str">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
@@ -951,10 +963,13 @@
       </c>
       <c r="E19" s="14"/>
     </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="10" t="str">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
@@ -962,10 +977,13 @@
       </c>
       <c r="E20" s="14"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="10" t="str">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
@@ -973,7 +991,7 @@
       </c>
       <c r="E21" s="14"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -989,7 +1007,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1005,7 +1023,7 @@
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1021,7 +1039,7 @@
       </c>
       <c r="E24" s="14"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1035,7 +1053,7 @@
       </c>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1046,7 +1064,7 @@
       </c>
       <c r="E26" s="15"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
updtae task velocity file
</commit_message>
<xml_diff>
--- a/ParcodeTaskVelocity.xlsx
+++ b/ParcodeTaskVelocity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\AWb-g4-parcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F55126-E7FE-4D7D-A36C-BB8F4719155F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B0A8C-49D7-4447-BE6E-668181814E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7501AF-60F9-49EB-99C2-B40735EA6386}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,7 +794,7 @@
       <c r="E8" s="7"/>
       <c r="H8">
         <f>SUM(Tableau1[Task velocity])/COUNT(Tableau1[Task velocity])</f>
-        <v>1.149098124098124</v>
+        <v>1.14512987012987</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1056,11 +1056,11 @@
         <v>10</v>
       </c>
       <c r="C25" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1.1111111111111112</v>
+        <v>1</v>
       </c>
       <c r="E25" s="7"/>
     </row>

</xml_diff>

<commit_message>
update TeskVelocity for Code Review
</commit_message>
<xml_diff>
--- a/ParcodeTaskVelocity.xlsx
+++ b/ParcodeTaskVelocity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\AWb-g4-parcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B0A8C-49D7-4447-BE6E-668181814E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DCCE9C-CBF2-4996-B797-8AC53780BBA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2171833D-4487-41F8-90D0-01F04C2BD05F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Tâche</t>
   </si>
@@ -110,9 +110,6 @@
     <t>suppression d'un commentaires</t>
   </si>
   <si>
-    <t>vue commentaire (ajout à la vue d'un code)</t>
-  </si>
-  <si>
     <t>mettre a jour contrôleur code pour ajouter un commentaire (ajout à la vue d'un code)</t>
   </si>
   <si>
@@ -159,6 +156,33 @@
   </si>
   <si>
     <t>ajouter une mini barre de navigation</t>
+  </si>
+  <si>
+    <t>AutoDoc d'une classe</t>
+  </si>
+  <si>
+    <t>TestUnitaire</t>
+  </si>
+  <si>
+    <t>Manuel Utilisateur</t>
+  </si>
+  <si>
+    <t>Revue de Codes - CSS</t>
+  </si>
+  <si>
+    <t>Revue de Code - JS</t>
+  </si>
+  <si>
+    <t>Revue de Codes -HTML</t>
+  </si>
+  <si>
+    <t>Revue de codes -PHP Models</t>
+  </si>
+  <si>
+    <t>Revues deCodes -PHP Controllers</t>
+  </si>
+  <si>
+    <t>Revue de Codes reste</t>
   </si>
 </sst>
 </file>
@@ -311,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E31" totalsRowShown="0">
-  <autoFilter ref="A1:E31" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B3A82C7C-2F49-4D69-AFEC-C86472461AEC}" name="Tableau1" displayName="Tableau1" ref="A1:E39" totalsRowShown="0">
+  <autoFilter ref="A1:E39" xr:uid="{F5F85825-DB6E-4F71-8F57-5392C2FDDCC0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
     <sortCondition ref="A1:A11"/>
   </sortState>
@@ -626,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C7501AF-60F9-49EB-99C2-B40735EA6386}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +887,7 @@
     </row>
     <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -911,12 +935,17 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>4</v>
+      </c>
+      <c r="D16" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>0.5</v>
       </c>
       <c r="E16" s="7"/>
     </row>
@@ -928,11 +957,11 @@
         <v>2</v>
       </c>
       <c r="C17" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E17" s="7"/>
     </row>
@@ -941,46 +970,46 @@
         <v>28</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D18" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12</v>
+      </c>
+      <c r="D19" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="D19" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1.2</v>
-      </c>
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="B20">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C20" s="2">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D20" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.83333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E20" s="14"/>
     </row>
@@ -989,30 +1018,30 @@
         <v>30</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="E21" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C22" s="2">
         <v>0.5</v>
       </c>
       <c r="D22" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="7"/>
     </row>
@@ -1021,62 +1050,60 @@
         <v>32</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D23" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v>1</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D24" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v>1</v>
       </c>
-      <c r="E24" s="14"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B25">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D25" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v>1</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B26">
-        <v>15</v>
-      </c>
-      <c r="C26" s="2">
-        <v>15</v>
-      </c>
-      <c r="D26" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E26" s="15"/>
     </row>
@@ -1085,24 +1112,26 @@
         <v>37</v>
       </c>
       <c r="B27">
-        <v>20</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="10" t="str">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v/>
-      </c>
-      <c r="E27" s="15"/>
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="10">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v>1</v>
+      </c>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B28">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C28" s="2">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D28" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
@@ -1115,30 +1144,30 @@
         <v>39</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C29" s="2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="D29" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
         <v>1</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B30">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D30" s="10">
         <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="E30" s="7"/>
     </row>
@@ -1147,16 +1176,126 @@
         <v>41</v>
       </c>
       <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="D31" s="10">
-        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
-        <v>1.3333333333333333</v>
+        <v>0.25</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
       </c>
       <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E34" s="7"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35">
+        <v>0.5</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36">
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E36" s="7"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E38" s="7"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="10" t="str">
+        <f>IFERROR(Tableau1[[#This Row],[Temps (estimation)]]/Tableau1[[#This Row],[Temps (réel)]], "")</f>
+        <v/>
+      </c>
+      <c r="E39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>